<commit_message>
Added function to calculate nextFinStatID and simplified the code flow in the tools.py file.
</commit_message>
<xml_diff>
--- a/guestLists/guestListID_register.xlsx
+++ b/guestLists/guestListID_register.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>guestListID_register</t>
   </si>
@@ -23,6 +23,30 @@
   </si>
   <si>
     <t>2021092002</t>
+  </si>
+  <si>
+    <t>2021092003</t>
+  </si>
+  <si>
+    <t>2021092004</t>
+  </si>
+  <si>
+    <t>2021092005</t>
+  </si>
+  <si>
+    <t>2021092006</t>
+  </si>
+  <si>
+    <t>2021092007</t>
+  </si>
+  <si>
+    <t>2021092008</t>
+  </si>
+  <si>
+    <t>G2021092001</t>
+  </si>
+  <si>
+    <t>G2021092002</t>
   </si>
 </sst>
 </file>
@@ -380,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -407,6 +431,70 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>